<commit_message>
advancing to the next tier
</commit_message>
<xml_diff>
--- a/all_words.xlsx
+++ b/all_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_PythonProjects\FinnishWordsLearner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A62A34-D05B-4AE3-86F5-A185F227ED61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499120E7-6134-4B27-98FF-35F1747466AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37590" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,16 +31,16 @@
     <t>Score</t>
   </si>
   <si>
+    <t>miettiä</t>
+  </si>
+  <si>
+    <t>to think (over), to consider</t>
+  </si>
+  <si>
     <t>jossain</t>
   </si>
   <si>
     <t>somewhere</t>
-  </si>
-  <si>
-    <t>miettiä</t>
-  </si>
-  <si>
-    <t>to think (over), to consider</t>
   </si>
   <si>
     <t>jotka</t>
@@ -4501,7 +4501,7 @@
   <dimension ref="A1:C704"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4525,7 +4525,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -4547,7 +4547,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4558,7 +4558,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -4569,7 +4569,7 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ui is more symmetric
</commit_message>
<xml_diff>
--- a/all_words.xlsx
+++ b/all_words.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -483,31 +483,31 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>jotka</t>
+          <t>jossain</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>who/that/which (relative)</t>
+          <t>somewhere</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>jossain</t>
+          <t>jotka</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>somewhere</t>
+          <t>who/that/which (relative)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -537,82 +537,82 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>päivällinen</t>
+          <t>tyhjä</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>dinner</t>
+          <t>empty</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>annos</t>
+          <t>yhtään</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>portion, dish</t>
+          <t>any (at all)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>keittiö</t>
+          <t>virhe</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>kitchen</t>
+          <t>mistake, error</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>timantti</t>
+          <t>päivällinen</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>diamond</t>
+          <t>dinner</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>virhe</t>
+          <t>timantti</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>mistake, error</t>
+          <t>diamond</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -642,157 +642,157 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ruuhka</t>
+          <t>kenkä</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>traffic jam</t>
+          <t>shoe</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>auttaa</t>
+          <t>näytelmä</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>to help</t>
+          <t>play (theatre)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>kenkä</t>
+          <t>olut</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>shoe</t>
+          <t>beer</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>yliopisto</t>
+          <t>keskusta</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>university</t>
+          <t>city center</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>keskusta</t>
+          <t>asukas</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>city center</t>
+          <t>inhabitant</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>asukas</t>
+          <t>keittiö</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>inhabitant</t>
+          <t>kitchen</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>yhtään</t>
+          <t>ruuhka</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>any (at all)</t>
+          <t>traffic jam</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>tyhjä</t>
+          <t>annos</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>empty</t>
+          <t>portion, dish</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>näytelmä</t>
+          <t>auttaa</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>play (theatre)</t>
+          <t>to help</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>olut</t>
+          <t>yliopisto</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>beer</t>
+          <t>university</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
UI || new columns Total/Left
</commit_message>
<xml_diff>
--- a/all_words.xlsx
+++ b/all_words.xlsx
@@ -5223,12 +5223,12 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>liha</t>
+          <t>ihminen</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>meat</t>
+          <t>human</t>
         </is>
       </c>
       <c r="C320" t="n">
@@ -5238,12 +5238,12 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>ihminen</t>
+          <t>hyvin</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>human</t>
+          <t>well (adverb)</t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -5253,12 +5253,12 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>hyvin</t>
+          <t>sohva</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>well (adverb)</t>
+          <t>sofa</t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -5268,12 +5268,12 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>sohva</t>
+          <t>kanadalainen</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>sofa</t>
+          <t>Canadian (adjective)</t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -5283,12 +5283,12 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>kanadalainen</t>
+          <t>puraista</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Canadian (adjective)</t>
+          <t>to bite</t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -5298,12 +5298,12 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>puraista</t>
+          <t>omena</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>to bite</t>
+          <t>apple</t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -5313,12 +5313,12 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>omena</t>
+          <t>korvapuusti</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>apple</t>
+          <t>cinnamon roll</t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -5328,12 +5328,12 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>korvapuusti</t>
+          <t>edes</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>cinnamon roll</t>
+          <t>even</t>
         </is>
       </c>
       <c r="C327" t="n">
@@ -5343,12 +5343,12 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>edes</t>
+          <t>ehkä</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>maybe</t>
         </is>
       </c>
       <c r="C328" t="n">
@@ -5358,12 +5358,12 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>ehkä</t>
+          <t>kasvi</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>maybe</t>
+          <t>plant</t>
         </is>
       </c>
       <c r="C329" t="n">
@@ -5373,12 +5373,12 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>kasvi</t>
+          <t>onnellinen</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>plant</t>
+          <t>happy</t>
         </is>
       </c>
       <c r="C330" t="n">
@@ -5388,12 +5388,12 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>onnellinen</t>
+          <t>litra</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>liter</t>
         </is>
       </c>
       <c r="C331" t="n">
@@ -5403,12 +5403,12 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>litra</t>
+          <t>Pariisi</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>liter</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="C332" t="n">
@@ -5418,12 +5418,12 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Pariisi</t>
+          <t>kilo</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>kilogram</t>
         </is>
       </c>
       <c r="C333" t="n">
@@ -5433,12 +5433,12 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>kilo</t>
+          <t>poikaystävä</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>kilogram</t>
+          <t>boyfriend</t>
         </is>
       </c>
       <c r="C334" t="n">
@@ -5448,12 +5448,12 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>poikaystävä</t>
+          <t>suomalainen</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>boyfriend</t>
+          <t>Finnish person</t>
         </is>
       </c>
       <c r="C335" t="n">
@@ -5463,12 +5463,12 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>suomalainen</t>
+          <t>onni</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>Finnish person</t>
+          <t>happiness</t>
         </is>
       </c>
       <c r="C336" t="n">
@@ -5478,12 +5478,12 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>onni</t>
+          <t>nämä</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>these</t>
         </is>
       </c>
       <c r="C337" t="n">
@@ -5493,12 +5493,12 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>nämä</t>
+          <t>vaari</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>these</t>
+          <t>grandpa</t>
         </is>
       </c>
       <c r="C338" t="n">
@@ -5508,12 +5508,12 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>vaari</t>
+          <t>karjalanpiirakka</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>grandpa</t>
+          <t>Karelian pasty</t>
         </is>
       </c>
       <c r="C339" t="n">
@@ -5523,12 +5523,12 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>karjalanpiirakka</t>
+          <t>saksa</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>Karelian pasty</t>
+          <t>German language</t>
         </is>
       </c>
       <c r="C340" t="n">
@@ -5538,12 +5538,12 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>saksa</t>
+          <t>myös</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>German language</t>
+          <t>also</t>
         </is>
       </c>
       <c r="C341" t="n">
@@ -5553,12 +5553,12 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>myös</t>
+          <t>kyllä</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>also</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="C342" t="n">
@@ -5568,12 +5568,12 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>insinööri</t>
+          <t>kana</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>engineer</t>
+          <t>chicken</t>
         </is>
       </c>
       <c r="C343" t="n">
@@ -5583,12 +5583,12 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>kyllä</t>
+          <t>laulaja</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>singer</t>
         </is>
       </c>
       <c r="C344" t="n">
@@ -5598,12 +5598,12 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>kana</t>
+          <t>sokeri</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>chicken</t>
+          <t>sugar</t>
         </is>
       </c>
       <c r="C345" t="n">
@@ -5613,12 +5613,12 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>laulaja</t>
+          <t>viisi</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>singer</t>
+          <t>five</t>
         </is>
       </c>
       <c r="C346" t="n">
@@ -5628,12 +5628,12 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>sokeri</t>
+          <t>tajuta</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>sugar</t>
+          <t>to realize</t>
         </is>
       </c>
       <c r="C347" t="n">
@@ -5643,12 +5643,12 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>viisi</t>
+          <t>tähti</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>five</t>
+          <t>star</t>
         </is>
       </c>
       <c r="C348" t="n">
@@ -5658,12 +5658,12 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>tajuta</t>
+          <t>ahma</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>to realize</t>
+          <t>wolwerine</t>
         </is>
       </c>
       <c r="C349" t="n">
@@ -5673,12 +5673,12 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>tähti</t>
+          <t>valkoinen</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>star</t>
+          <t>white</t>
         </is>
       </c>
       <c r="C350" t="n">
@@ -5688,12 +5688,12 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>ahma</t>
+          <t>karhu</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>wolwerine</t>
+          <t>bear</t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -5703,12 +5703,12 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>valkoinen</t>
+          <t>kellari</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>white</t>
+          <t>basement</t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -5718,12 +5718,12 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>karhu</t>
+          <t>Elsa</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>bear</t>
+          <t>Elsa</t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -5733,12 +5733,12 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>kellari</t>
+          <t>he</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>basement</t>
+          <t>they</t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -5748,12 +5748,12 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Elsa</t>
+          <t>susi</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>Elsa</t>
+          <t>wolf</t>
         </is>
       </c>
       <c r="C355" t="n">
@@ -5763,12 +5763,12 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>he</t>
+          <t>kaupunki</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>they</t>
+          <t>city</t>
         </is>
       </c>
       <c r="C356" t="n">
@@ -5778,12 +5778,12 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>susi</t>
+          <t>morsian</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>wolf</t>
+          <t>bride</t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -5793,12 +5793,12 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>kaupunki</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>city</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -5808,12 +5808,12 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>morsian</t>
+          <t>afrikkalainen</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>bride</t>
+          <t>African</t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -5823,12 +5823,12 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>peli</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>game</t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -5838,12 +5838,12 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>afrikkalainen</t>
+          <t>tosi</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>African</t>
+          <t>really (adverb of degree, spoken language)</t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -5853,12 +5853,12 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>peli</t>
+          <t>käärme</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>game</t>
+          <t>snake</t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -5868,12 +5868,12 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>tosi</t>
+          <t>kirjoittaa</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>really (adverb of degree, spoken language)</t>
+          <t>to write</t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -5883,12 +5883,12 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>käärme</t>
+          <t>koira</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>snake</t>
+          <t>dog</t>
         </is>
       </c>
       <c r="C364" t="n">
@@ -5898,12 +5898,12 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>kirjoittaa</t>
+          <t>Pyry</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>to write</t>
+          <t>Pyry</t>
         </is>
       </c>
       <c r="C365" t="n">
@@ -5913,12 +5913,12 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>koira</t>
+          <t>mukava</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>dog</t>
+          <t>comfortable</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -5928,12 +5928,12 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Pyry</t>
+          <t>Suomi</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>Pyry</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C367" t="n">
@@ -5943,12 +5943,12 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>mukava</t>
+          <t>ruotsalainen</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>comfortable</t>
+          <t>Swedish person</t>
         </is>
       </c>
       <c r="C368" t="n">
@@ -5958,12 +5958,12 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Suomi</t>
+          <t>herkullinen</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>delicious</t>
         </is>
       </c>
       <c r="C369" t="n">
@@ -5973,12 +5973,12 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>ruotsalainen</t>
+          <t>velho</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Swedish person</t>
+          <t>wizard</t>
         </is>
       </c>
       <c r="C370" t="n">
@@ -5988,12 +5988,12 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>herkullinen</t>
+          <t>ovat</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>delicious</t>
+          <t>(they) are</t>
         </is>
       </c>
       <c r="C371" t="n">
@@ -6003,12 +6003,12 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>velho</t>
+          <t>grilli</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>wizard</t>
+          <t>grill</t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -6018,12 +6018,12 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>ovat</t>
+          <t>pyöreä</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>(they) are</t>
+          <t>round</t>
         </is>
       </c>
       <c r="C373" t="n">
@@ -6033,12 +6033,12 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>grilli</t>
+          <t>kolme</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>grill</t>
+          <t>three</t>
         </is>
       </c>
       <c r="C374" t="n">
@@ -6048,12 +6048,12 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>pyöreä</t>
+          <t>tuo</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>round</t>
+          <t>that (adjective)</t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -6063,12 +6063,12 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>kolme</t>
+          <t>hän</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>three</t>
+          <t>s/he</t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -6078,12 +6078,12 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>tuo</t>
+          <t>itkeä</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>that (adjective)</t>
+          <t>to cry</t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -6093,12 +6093,12 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>hän</t>
+          <t>tanskalainen</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>s/he</t>
+          <t>Danish person</t>
         </is>
       </c>
       <c r="C378" t="n">
@@ -6108,12 +6108,12 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>itkeä</t>
+          <t>makkara</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>to cry</t>
+          <t>sausage</t>
         </is>
       </c>
       <c r="C379" t="n">
@@ -6123,12 +6123,12 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>tanskalainen</t>
+          <t>jotain</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>Danish person</t>
+          <t>something</t>
         </is>
       </c>
       <c r="C380" t="n">
@@ -6138,12 +6138,12 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>makkara</t>
+          <t>sinivalkoinen</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>sausage</t>
+          <t>blue and white</t>
         </is>
       </c>
       <c r="C381" t="n">
@@ -6153,12 +6153,12 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>jotain</t>
+          <t>loppu</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>something</t>
+          <t>out of</t>
         </is>
       </c>
       <c r="C382" t="n">
@@ -6168,12 +6168,12 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>sinivalkoinen</t>
+          <t>espanja</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>blue and white</t>
+          <t>Spanish language</t>
         </is>
       </c>
       <c r="C383" t="n">
@@ -6183,12 +6183,12 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>loppu</t>
+          <t>kuusi</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>out of</t>
+          <t>spruce</t>
         </is>
       </c>
       <c r="C384" t="n">
@@ -6198,12 +6198,12 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>espanja</t>
+          <t>väärin</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>Spanish language</t>
+          <t>incorrect (adverb)</t>
         </is>
       </c>
       <c r="C385" t="n">
@@ -6213,12 +6213,12 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>kuusi</t>
+          <t>jo</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>spruce</t>
+          <t>already</t>
         </is>
       </c>
       <c r="C386" t="n">
@@ -6228,12 +6228,12 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>väärin</t>
+          <t>aika</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>incorrect (adverb)</t>
+          <t>time</t>
         </is>
       </c>
       <c r="C387" t="n">
@@ -6243,12 +6243,12 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>jo</t>
+          <t>mämmi</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>already</t>
+          <t>mämmi</t>
         </is>
       </c>
       <c r="C388" t="n">
@@ -6258,12 +6258,12 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>aika</t>
+          <t>opettaja</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>time</t>
+          <t>teacher</t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -6273,12 +6273,12 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>mämmi</t>
+          <t>tyttöystävä</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>mämmi</t>
+          <t>girlfriend</t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -6288,12 +6288,12 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>opettaja</t>
+          <t>hevonen</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>teacher</t>
+          <t>horse</t>
         </is>
       </c>
       <c r="C391" t="n">
@@ -6303,12 +6303,12 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>tyttöystävä</t>
+          <t>Oslo</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>girlfriend</t>
+          <t>Oslo</t>
         </is>
       </c>
       <c r="C392" t="n">
@@ -6318,12 +6318,12 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>hevonen</t>
+          <t>oikea</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>horse</t>
+          <t>right (adjective)</t>
         </is>
       </c>
       <c r="C393" t="n">
@@ -6333,12 +6333,12 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>-kä</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>nor</t>
         </is>
       </c>
       <c r="C394" t="n">
@@ -6348,12 +6348,12 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>oikea</t>
+          <t>kaukana</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>right (adjective)</t>
+          <t>far away</t>
         </is>
       </c>
       <c r="C395" t="n">
@@ -6363,12 +6363,12 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>-kä</t>
+          <t>missä</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>nor</t>
+          <t>where</t>
         </is>
       </c>
       <c r="C396" t="n">
@@ -6378,12 +6378,12 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>kaukana</t>
+          <t>vielä</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>far away</t>
+          <t>still</t>
         </is>
       </c>
       <c r="C397" t="n">
@@ -6393,12 +6393,12 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>missä</t>
+          <t>akku</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>where</t>
+          <t>battery</t>
         </is>
       </c>
       <c r="C398" t="n">
@@ -6408,12 +6408,12 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>vielä</t>
+          <t>vadelma</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>still</t>
+          <t>raspberry</t>
         </is>
       </c>
       <c r="C399" t="n">
@@ -6423,12 +6423,12 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>akku</t>
+          <t>puoli</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>battery</t>
+          <t>half</t>
         </is>
       </c>
       <c r="C400" t="n">
@@ -6438,12 +6438,12 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>vadelma</t>
+          <t>hindi</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>raspberry</t>
+          <t>Hindi (language)</t>
         </is>
       </c>
       <c r="C401" t="n">
@@ -6453,12 +6453,12 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>puoli</t>
+          <t>ketkä</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>half</t>
+          <t>who (are the people)</t>
         </is>
       </c>
       <c r="C402" t="n">
@@ -6468,12 +6468,12 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>hindi</t>
+          <t>pehmeä</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>Hindi (language)</t>
+          <t>soft</t>
         </is>
       </c>
       <c r="C403" t="n">
@@ -6483,12 +6483,12 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>ketkä</t>
+          <t>voi voi</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>who (are the people)</t>
+          <t>oh dear (~butter)</t>
         </is>
       </c>
       <c r="C404" t="n">
@@ -6498,12 +6498,12 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>pehmeä</t>
+          <t>kaikki</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>soft</t>
+          <t>everyone</t>
         </is>
       </c>
       <c r="C405" t="n">
@@ -6513,12 +6513,12 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>voi voi</t>
+          <t>laturi</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>oh dear (~butter)</t>
+          <t>charger</t>
         </is>
       </c>
       <c r="C406" t="n">
@@ -6528,12 +6528,12 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>kaikki</t>
+          <t>kuin</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>everyone</t>
+          <t>as (comparison)</t>
         </is>
       </c>
       <c r="C407" t="n">
@@ -6543,12 +6543,12 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>laturi</t>
+          <t>Skandinavia</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>charger</t>
+          <t>Skandinavia</t>
         </is>
       </c>
       <c r="C408" t="n">
@@ -6558,12 +6558,12 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>kuin</t>
+          <t>sauna</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>as (comparison)</t>
+          <t>sauna</t>
         </is>
       </c>
       <c r="C409" t="n">
@@ -6573,12 +6573,12 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>Skandinavia</t>
+          <t>sisu</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>Skandinavia</t>
+          <t>true grit</t>
         </is>
       </c>
       <c r="C410" t="n">
@@ -6588,12 +6588,12 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>sauna</t>
+          <t>kanadalainen</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>sauna</t>
+          <t>Canadian person</t>
         </is>
       </c>
       <c r="C411" t="n">
@@ -6603,12 +6603,12 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>sisu</t>
+          <t>radio</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>true grit</t>
+          <t>radio</t>
         </is>
       </c>
       <c r="C412" t="n">
@@ -6618,12 +6618,12 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>kanadalainen</t>
+          <t>ihahaa</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>Canadian person</t>
+          <t>neigh (horse sound)</t>
         </is>
       </c>
       <c r="C413" t="n">
@@ -6633,12 +6633,12 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>radio</t>
+          <t>netti</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>radio</t>
+          <t>net (IT)</t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -6648,12 +6648,12 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>ihahaa</t>
+          <t>murre</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>neigh (horse sound)</t>
+          <t>dialect</t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -6663,12 +6663,12 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>netti</t>
+          <t>tai</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>net (IT)</t>
+          <t>or (inclusive)</t>
         </is>
       </c>
       <c r="C416" t="n">
@@ -6678,12 +6678,12 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>murre</t>
+          <t>kirkas</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>dialect</t>
+          <t>bright</t>
         </is>
       </c>
       <c r="C417" t="n">
@@ -6693,12 +6693,12 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>tai</t>
+          <t>likainen</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>or (inclusive)</t>
+          <t>dirty</t>
         </is>
       </c>
       <c r="C418" t="n">
@@ -6708,12 +6708,12 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>kirkas</t>
+          <t>Kanada</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>bright</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="C419" t="n">
@@ -6723,12 +6723,12 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>likainen</t>
+          <t>vaikea</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>dirty</t>
+          <t>difficult</t>
         </is>
       </c>
       <c r="C420" t="n">
@@ -6738,12 +6738,12 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>Kanada</t>
+          <t>vaarallinen</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>dangerous</t>
         </is>
       </c>
       <c r="C421" t="n">
@@ -6753,12 +6753,12 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>vaikea</t>
+          <t>viisas</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>difficult</t>
+          <t>wise</t>
         </is>
       </c>
       <c r="C422" t="n">
@@ -6768,12 +6768,12 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>vaarallinen</t>
+          <t>kameli</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>dangerous</t>
+          <t>camel</t>
         </is>
       </c>
       <c r="C423" t="n">
@@ -6783,12 +6783,12 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>viisas</t>
+          <t>terve</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>wise</t>
+          <t>hello</t>
         </is>
       </c>
       <c r="C424" t="n">
@@ -6798,12 +6798,12 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>kameli</t>
+          <t>kiinni</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>camel</t>
+          <t>closed</t>
         </is>
       </c>
       <c r="C425" t="n">
@@ -6813,12 +6813,12 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>terve</t>
+          <t>miau</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>hello</t>
+          <t>meow (cat sound)</t>
         </is>
       </c>
       <c r="C426" t="n">
@@ -6828,12 +6828,12 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>kiinni</t>
+          <t>Viro</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>closed</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="C427" t="n">
@@ -6843,12 +6843,12 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>miau</t>
+          <t>naimisissa</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>meow (cat sound)</t>
+          <t>married</t>
         </is>
       </c>
       <c r="C428" t="n">
@@ -6858,12 +6858,12 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>Viro</t>
+          <t>oopperatalo</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>opera house</t>
         </is>
       </c>
       <c r="C429" t="n">
@@ -6873,12 +6873,12 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>naimisissa</t>
+          <t>onnea</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>married</t>
+          <t>good luck</t>
         </is>
       </c>
       <c r="C430" t="n">
@@ -6888,12 +6888,12 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>oopperatalo</t>
+          <t>kenguru</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>opera house</t>
+          <t>kangaroo</t>
         </is>
       </c>
       <c r="C431" t="n">
@@ -6903,12 +6903,12 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>onnea</t>
+          <t>monumentti</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>good luck</t>
+          <t>monument</t>
         </is>
       </c>
       <c r="C432" t="n">
@@ -6918,12 +6918,12 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>kenguru</t>
+          <t>sininen</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>kangaroo</t>
+          <t>blue</t>
         </is>
       </c>
       <c r="C433" t="n">
@@ -6933,12 +6933,12 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>monumentti</t>
+          <t>voida</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>monument</t>
+          <t>may, can, to be able to</t>
         </is>
       </c>
       <c r="C434" t="n">
@@ -6948,12 +6948,12 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>sininen</t>
+          <t>röh</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>blue</t>
+          <t>oink</t>
         </is>
       </c>
       <c r="C435" t="n">
@@ -6963,12 +6963,12 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>voida</t>
+          <t>nyt</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>may, can, to be able to</t>
+          <t>now</t>
         </is>
       </c>
       <c r="C436" t="n">
@@ -6978,12 +6978,12 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>röh</t>
+          <t>kiitos</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>oink</t>
+          <t>thank you</t>
         </is>
       </c>
       <c r="C437" t="n">
@@ -6993,12 +6993,12 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>nyt</t>
+          <t>au</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>now</t>
+          <t>ouch</t>
         </is>
       </c>
       <c r="C438" t="n">
@@ -7008,12 +7008,12 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>kiitos</t>
+          <t>myydä</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>thank you</t>
+          <t>to sell</t>
         </is>
       </c>
       <c r="C439" t="n">
@@ -7023,12 +7023,12 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>au</t>
+          <t>paljonko</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>ouch</t>
+          <t>how much</t>
         </is>
       </c>
       <c r="C440" t="n">
@@ -7038,12 +7038,12 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>myydä</t>
+          <t>veri</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>to sell</t>
+          <t>blood</t>
         </is>
       </c>
       <c r="C441" t="n">
@@ -7053,12 +7053,12 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>paljonko</t>
+          <t>mauste</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>how much</t>
+          <t>spice</t>
         </is>
       </c>
       <c r="C442" t="n">
@@ -7068,12 +7068,12 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>veri</t>
+          <t>oletko</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>blood</t>
+          <t>are (you singular in question)</t>
         </is>
       </c>
       <c r="C443" t="n">
@@ -7083,12 +7083,12 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>mauste</t>
+          <t>sima</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>spice</t>
+          <t>mead</t>
         </is>
       </c>
       <c r="C444" t="n">
@@ -7098,12 +7098,12 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>oletko</t>
+          <t>islantilainen</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
         <is>
-          <t>are (you singular in question)</t>
+          <t>Icelandic person</t>
         </is>
       </c>
       <c r="C445" t="n">
@@ -7113,12 +7113,12 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>sima</t>
+          <t>glögi</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
         <is>
-          <t>mead</t>
+          <t>glögi</t>
         </is>
       </c>
       <c r="C446" t="n">
@@ -7128,12 +7128,12 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>islantilainen</t>
+          <t>saamelainen</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
         <is>
-          <t>Icelandic person</t>
+          <t>Sámi person</t>
         </is>
       </c>
       <c r="C447" t="n">
@@ -7143,12 +7143,12 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>glögi</t>
+          <t>venäläinen</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
         <is>
-          <t>glögi</t>
+          <t>Russian person</t>
         </is>
       </c>
       <c r="C448" t="n">
@@ -7158,12 +7158,12 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>saamelainen</t>
+          <t>lemmikki</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
         <is>
-          <t>Sámi person</t>
+          <t>pet</t>
         </is>
       </c>
       <c r="C449" t="n">
@@ -7173,12 +7173,12 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>venäläinen</t>
+          <t>osata</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
         <is>
-          <t>Russian person</t>
+          <t>to know how to</t>
         </is>
       </c>
       <c r="C450" t="n">
@@ -7188,12 +7188,12 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>lemmikki</t>
+          <t>kuinka</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>pet</t>
+          <t>how</t>
         </is>
       </c>
       <c r="C451" t="n">
@@ -7203,12 +7203,12 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>osata</t>
+          <t>limonadi</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
         <is>
-          <t>to know how to</t>
+          <t>soda pop</t>
         </is>
       </c>
       <c r="C452" t="n">
@@ -7218,12 +7218,12 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>kuinka</t>
+          <t>koko</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
         <is>
-          <t>how</t>
+          <t>the whole</t>
         </is>
       </c>
       <c r="C453" t="n">
@@ -7233,12 +7233,12 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>limonadi</t>
+          <t>murista</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
         <is>
-          <t>soda pop</t>
+          <t>to growl</t>
         </is>
       </c>
       <c r="C454" t="n">
@@ -7248,12 +7248,12 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>koko</t>
+          <t>lämmin</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>the whole</t>
+          <t>warm</t>
         </is>
       </c>
       <c r="C455" t="n">
@@ -7263,12 +7263,12 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>murista</t>
+          <t>olla ikävä</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
         <is>
-          <t>to growl</t>
+          <t>to miss</t>
         </is>
       </c>
       <c r="C456" t="n">
@@ -7278,12 +7278,12 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>lämmin</t>
+          <t>Berliini</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
         <is>
-          <t>warm</t>
+          <t>Berlin</t>
         </is>
       </c>
       <c r="C457" t="n">
@@ -7293,12 +7293,12 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>olla ikävä</t>
+          <t>sulaa</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
         <is>
-          <t>to miss</t>
+          <t>to melt</t>
         </is>
       </c>
       <c r="C458" t="n">
@@ -7308,12 +7308,12 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>Berliini</t>
+          <t>ruoka</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>Berlin</t>
+          <t>food</t>
         </is>
       </c>
       <c r="C459" t="n">
@@ -7323,12 +7323,12 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>sulaa</t>
+          <t>jolla</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>to melt</t>
+          <t>who/which (has) (relative)</t>
         </is>
       </c>
       <c r="C460" t="n">
@@ -7338,12 +7338,12 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>ruoka</t>
+          <t>auki</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
         <is>
-          <t>food</t>
+          <t>open</t>
         </is>
       </c>
       <c r="C461" t="n">
@@ -7353,12 +7353,12 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>jolla</t>
+          <t>nopeasti</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>who/which (has) (relative)</t>
+          <t>quickly</t>
         </is>
       </c>
       <c r="C462" t="n">
@@ -7368,12 +7368,12 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>auki</t>
+          <t>Islanti</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>open</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="C463" t="n">
@@ -7383,12 +7383,12 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>nopeasti</t>
+          <t>nauraa</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>quickly</t>
+          <t>to laugh</t>
         </is>
       </c>
       <c r="C464" t="n">
@@ -7398,12 +7398,12 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>Islanti</t>
+          <t>Tyyne</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Tyyne</t>
         </is>
       </c>
       <c r="C465" t="n">
@@ -7413,12 +7413,12 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>nauraa</t>
+          <t>rahka</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>to laugh</t>
+          <t>quark</t>
         </is>
       </c>
       <c r="C466" t="n">
@@ -7428,12 +7428,12 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>Tyyne</t>
+          <t>stadion</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>Tyyne</t>
+          <t>stadium</t>
         </is>
       </c>
       <c r="C467" t="n">
@@ -7443,12 +7443,12 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>rahka</t>
+          <t>kahdeksan</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>quark</t>
+          <t>eight</t>
         </is>
       </c>
       <c r="C468" t="n">
@@ -7458,12 +7458,12 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>stadion</t>
+          <t>pupu</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>stadium</t>
+          <t>bunny</t>
         </is>
       </c>
       <c r="C469" t="n">
@@ -7473,12 +7473,12 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>kahdeksan</t>
+          <t>tuhma</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>eight</t>
+          <t>naughty</t>
         </is>
       </c>
       <c r="C470" t="n">
@@ -7488,12 +7488,12 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>pupu</t>
+          <t>marja</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>bunny</t>
+          <t>berry</t>
         </is>
       </c>
       <c r="C471" t="n">
@@ -7503,12 +7503,12 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>tuhma</t>
+          <t>hauska</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>naughty</t>
+          <t>funny</t>
         </is>
       </c>
       <c r="C472" t="n">
@@ -7518,12 +7518,12 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>marja</t>
+          <t>sydän</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>berry</t>
+          <t>heart</t>
         </is>
       </c>
       <c r="C473" t="n">
@@ -7533,12 +7533,12 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>hauska</t>
+          <t>taas</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>funny</t>
+          <t>again</t>
         </is>
       </c>
       <c r="C474" t="n">
@@ -7548,12 +7548,12 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>sydän</t>
+          <t>meri</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>heart</t>
+          <t>sea</t>
         </is>
       </c>
       <c r="C475" t="n">
@@ -7563,12 +7563,12 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>taas</t>
+          <t>lehti</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>again</t>
+          <t>leaf</t>
         </is>
       </c>
       <c r="C476" t="n">
@@ -7578,12 +7578,12 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>meri</t>
+          <t>auto</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>sea</t>
+          <t>car</t>
         </is>
       </c>
       <c r="C477" t="n">
@@ -7593,12 +7593,12 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>lehti</t>
+          <t>varma</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>leaf</t>
+          <t>sure, certain</t>
         </is>
       </c>
       <c r="C478" t="n">
@@ -7608,12 +7608,12 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>auto</t>
+          <t>sama</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>same</t>
         </is>
       </c>
       <c r="C479" t="n">
@@ -7623,12 +7623,12 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>varma</t>
+          <t>minuutti</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>sure, certain</t>
+          <t>minute</t>
         </is>
       </c>
       <c r="C480" t="n">
@@ -7638,12 +7638,12 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>sama</t>
+          <t>korea</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>same</t>
+          <t>Korean language</t>
         </is>
       </c>
       <c r="C481" t="n">
@@ -7653,12 +7653,12 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>minuutti</t>
+          <t>kivi</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>minute</t>
+          <t>stone, rock</t>
         </is>
       </c>
       <c r="C482" t="n">
@@ -7668,12 +7668,12 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>korea</t>
+          <t>kai</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>Korean language</t>
+          <t>maybe, I guess</t>
         </is>
       </c>
       <c r="C483" t="n">
@@ -7683,12 +7683,12 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>kivi</t>
+          <t>yrittää</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>stone, rock</t>
+          <t>to try</t>
         </is>
       </c>
       <c r="C484" t="n">
@@ -7698,12 +7698,12 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>kai</t>
+          <t>älykäs</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>maybe, I guess</t>
+          <t>intelligent</t>
         </is>
       </c>
       <c r="C485" t="n">
@@ -7713,12 +7713,12 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>yrittää</t>
+          <t>metsä</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>to try</t>
+          <t>forest</t>
         </is>
       </c>
       <c r="C486" t="n">
@@ -7728,12 +7728,12 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>älykäs</t>
+          <t>poika</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>intelligent</t>
+          <t>boy</t>
         </is>
       </c>
       <c r="C487" t="n">
@@ -7743,12 +7743,12 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>metsä</t>
+          <t>tabletti</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>tablet</t>
         </is>
       </c>
       <c r="C488" t="n">
@@ -7758,12 +7758,12 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>poika</t>
+          <t>juosta</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>boy</t>
+          <t>to run</t>
         </is>
       </c>
       <c r="C489" t="n">
@@ -7773,12 +7773,12 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>tabletti</t>
+          <t>mummo</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>tablet</t>
+          <t>grandma</t>
         </is>
       </c>
       <c r="C490" t="n">
@@ -7788,12 +7788,12 @@
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>juosta</t>
+          <t>suklaa</t>
         </is>
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>to run</t>
+          <t>chocolate</t>
         </is>
       </c>
       <c r="C491" t="n">
@@ -7803,12 +7803,12 @@
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>mummo</t>
+          <t>hei</t>
         </is>
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>grandma</t>
+          <t>hi (greeting)</t>
         </is>
       </c>
       <c r="C492" t="n">
@@ -7818,12 +7818,12 @@
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>suklaa</t>
+          <t>kiisseli</t>
         </is>
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>chocolate</t>
+          <t>kissel</t>
         </is>
       </c>
       <c r="C493" t="n">
@@ -7833,12 +7833,12 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>hei</t>
+          <t>syötävä</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>hi (greeting)</t>
+          <t>edible</t>
         </is>
       </c>
       <c r="C494" t="n">
@@ -7848,12 +7848,12 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>kiisseli</t>
+          <t>uusi</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>kissel</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C495" t="n">
@@ -7863,12 +7863,12 @@
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>syötävä</t>
+          <t>karkki</t>
         </is>
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>edible</t>
+          <t>candy</t>
         </is>
       </c>
       <c r="C496" t="n">
@@ -7878,12 +7878,12 @@
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>uusi</t>
+          <t>kantele</t>
         </is>
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>kantele</t>
         </is>
       </c>
       <c r="C497" t="n">
@@ -7893,12 +7893,12 @@
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>karkki</t>
+          <t>ranska</t>
         </is>
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>candy</t>
+          <t>French language</t>
         </is>
       </c>
       <c r="C498" t="n">
@@ -7908,12 +7908,12 @@
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>kantele</t>
+          <t>haarukka</t>
         </is>
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>kantele</t>
+          <t>fork</t>
         </is>
       </c>
       <c r="C499" t="n">
@@ -7923,12 +7923,12 @@
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>ranska</t>
+          <t>vihreä</t>
         </is>
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>French language</t>
+          <t>green</t>
         </is>
       </c>
       <c r="C500" t="n">
@@ -7938,12 +7938,12 @@
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>haarukka</t>
+          <t>komea</t>
         </is>
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>fork</t>
+          <t>handsome</t>
         </is>
       </c>
       <c r="C501" t="n">
@@ -7953,12 +7953,12 @@
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>vihreä</t>
+          <t>viettää</t>
         </is>
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>green</t>
+          <t>to spend (time, vacation)</t>
         </is>
       </c>
       <c r="C502" t="n">
@@ -7968,12 +7968,12 @@
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>komea</t>
+          <t>monta</t>
         </is>
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>handsome</t>
+          <t>many (partitive)</t>
         </is>
       </c>
       <c r="C503" t="n">
@@ -7983,12 +7983,12 @@
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>viettää</t>
+          <t>kiltti</t>
         </is>
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>to spend (time, vacation)</t>
+          <t>well-behaved</t>
         </is>
       </c>
       <c r="C504" t="n">
@@ -7998,12 +7998,12 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>monta</t>
+          <t>tasan</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>many (partitive)</t>
+          <t>even, exactly (time)</t>
         </is>
       </c>
       <c r="C505" t="n">
@@ -8013,12 +8013,12 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>kiltti</t>
+          <t>kuppi</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>well-behaved</t>
+          <t>cup (of)</t>
         </is>
       </c>
       <c r="C506" t="n">
@@ -8028,12 +8028,12 @@
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>tasan</t>
+          <t>kartta</t>
         </is>
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>even, exactly (time)</t>
+          <t>map</t>
         </is>
       </c>
       <c r="C507" t="n">
@@ -8043,12 +8043,12 @@
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>kuppi</t>
+          <t>Lontoo</t>
         </is>
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>cup (of)</t>
+          <t>London</t>
         </is>
       </c>
       <c r="C508" t="n">
@@ -8058,12 +8058,12 @@
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>kartta</t>
+          <t>Italia</t>
         </is>
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>map</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C509" t="n">
@@ -8073,12 +8073,12 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>Lontoo</t>
+          <t>ahkera</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>hardworking</t>
         </is>
       </c>
       <c r="C510" t="n">
@@ -8088,12 +8088,12 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>Italia</t>
+          <t>koti-ikävä</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>home sickness</t>
         </is>
       </c>
       <c r="C511" t="n">
@@ -8103,12 +8103,12 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>ahkera</t>
+          <t>banaani</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>hardworking</t>
+          <t>banana</t>
         </is>
       </c>
       <c r="C512" t="n">
@@ -8118,12 +8118,12 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>koti-ikävä</t>
+          <t>olette</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>home sickness</t>
+          <t>(you plural) are</t>
         </is>
       </c>
       <c r="C513" t="n">
@@ -8133,12 +8133,12 @@
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>banaani</t>
+          <t>suolainen</t>
         </is>
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>banana</t>
+          <t>salty, savory</t>
         </is>
       </c>
       <c r="C514" t="n">
@@ -8148,12 +8148,12 @@
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>olette</t>
+          <t>lattia</t>
         </is>
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>(you plural) are</t>
+          <t>floor (the type you stand on)</t>
         </is>
       </c>
       <c r="C515" t="n">
@@ -8163,12 +8163,12 @@
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>suolainen</t>
+          <t>juotava</t>
         </is>
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>salty, savory</t>
+          <t>drinkable</t>
         </is>
       </c>
       <c r="C516" t="n">
@@ -8178,12 +8178,12 @@
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>lattia</t>
+          <t>lehmä</t>
         </is>
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>floor (the type you stand on)</t>
+          <t>cow</t>
         </is>
       </c>
       <c r="C517" t="n">
@@ -8193,12 +8193,12 @@
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>juotava</t>
+          <t>mukava</t>
         </is>
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>drinkable</t>
+          <t>nice</t>
         </is>
       </c>
       <c r="C518" t="n">
@@ -8208,12 +8208,12 @@
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>lehmä</t>
+          <t>istua</t>
         </is>
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>cow</t>
+          <t>to sit</t>
         </is>
       </c>
       <c r="C519" t="n">
@@ -8223,12 +8223,12 @@
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t>mukava</t>
+          <t>virolainen</t>
         </is>
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>nice</t>
+          <t>Estonian person</t>
         </is>
       </c>
       <c r="C520" t="n">
@@ -8238,12 +8238,12 @@
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>istua</t>
+          <t>melkein</t>
         </is>
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>to sit</t>
+          <t>almost</t>
         </is>
       </c>
       <c r="C521" t="n">
@@ -8253,12 +8253,12 @@
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>virolainen</t>
+          <t>sillä</t>
         </is>
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>Estonian person</t>
+          <t>(it) has</t>
         </is>
       </c>
       <c r="C522" t="n">
@@ -8268,12 +8268,12 @@
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>melkein</t>
+          <t>juoda</t>
         </is>
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>almost</t>
+          <t>to drink</t>
         </is>
       </c>
       <c r="C523" t="n">
@@ -8283,12 +8283,12 @@
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>sillä</t>
+          <t>sana</t>
         </is>
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>(it) has</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C524" t="n">
@@ -8298,12 +8298,12 @@
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>juoda</t>
+          <t>harmaa</t>
         </is>
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>to drink</t>
+          <t>grey</t>
         </is>
       </c>
       <c r="C525" t="n">
@@ -8313,12 +8313,12 @@
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>sana</t>
+          <t>väärä</t>
         </is>
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>word</t>
+          <t>wrong (adjective)</t>
         </is>
       </c>
       <c r="C526" t="n">
@@ -8328,12 +8328,12 @@
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>harmaa</t>
+          <t>seisoa</t>
         </is>
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>grey</t>
+          <t>to stand</t>
         </is>
       </c>
       <c r="C527" t="n">
@@ -8343,12 +8343,12 @@
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>väärä</t>
+          <t>pieni</t>
         </is>
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>wrong (adjective)</t>
+          <t>small</t>
         </is>
       </c>
       <c r="C528" t="n">
@@ -8358,12 +8358,12 @@
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>seisoa</t>
+          <t>salaatti</t>
         </is>
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>to stand</t>
+          <t>salad</t>
         </is>
       </c>
       <c r="C529" t="n">
@@ -8373,12 +8373,12 @@
     <row r="530">
       <c r="A530" t="inlineStr">
         <is>
-          <t>pieni</t>
+          <t>kahvi</t>
         </is>
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>small</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="C530" t="n">
@@ -8388,12 +8388,12 @@
     <row r="531">
       <c r="A531" t="inlineStr">
         <is>
-          <t>salaatti</t>
+          <t>paljonko</t>
         </is>
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>salad</t>
+          <t>what (time)</t>
         </is>
       </c>
       <c r="C531" t="n">
@@ -8403,12 +8403,12 @@
     <row r="532">
       <c r="A532" t="inlineStr">
         <is>
-          <t>kahvi</t>
+          <t>ihailla</t>
         </is>
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>to admire</t>
         </is>
       </c>
       <c r="C532" t="n">
@@ -8418,12 +8418,12 @@
     <row r="533">
       <c r="A533" t="inlineStr">
         <is>
-          <t>paljonko</t>
+          <t>kerma</t>
         </is>
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>what (time)</t>
+          <t>cream</t>
         </is>
       </c>
       <c r="C533" t="n">
@@ -8433,12 +8433,12 @@
     <row r="534">
       <c r="A534" t="inlineStr">
         <is>
-          <t>ihailla</t>
+          <t>siivota</t>
         </is>
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>to admire</t>
+          <t>to tidy up</t>
         </is>
       </c>
       <c r="C534" t="n">
@@ -8448,12 +8448,12 @@
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>kerma</t>
+          <t>keskellä</t>
         </is>
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>cream</t>
+          <t>in the middle of</t>
         </is>
       </c>
       <c r="C535" t="n">
@@ -8463,12 +8463,12 @@
     <row r="536">
       <c r="A536" t="inlineStr">
         <is>
-          <t>siivota</t>
+          <t>missä</t>
         </is>
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>to tidy up</t>
+          <t>where (relative)</t>
         </is>
       </c>
       <c r="C536" t="n">
@@ -8478,12 +8478,12 @@
     <row r="537">
       <c r="A537" t="inlineStr">
         <is>
-          <t>keskellä</t>
+          <t>nainen</t>
         </is>
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>in the middle of</t>
+          <t>woman</t>
         </is>
       </c>
       <c r="C537" t="n">
@@ -8493,12 +8493,12 @@
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t>missä</t>
+          <t>no</t>
         </is>
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>where (relative)</t>
+          <t>well (phrase)</t>
         </is>
       </c>
       <c r="C538" t="n">
@@ -8508,12 +8508,12 @@
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>nainen</t>
+          <t>ainakin</t>
         </is>
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>woman</t>
+          <t>at least</t>
         </is>
       </c>
       <c r="C539" t="n">
@@ -8523,12 +8523,12 @@
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>täydellinen</t>
         </is>
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>well (phrase)</t>
+          <t>perfect</t>
         </is>
       </c>
       <c r="C540" t="n">
@@ -8538,12 +8538,12 @@
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>ainakin</t>
+          <t>puisto</t>
         </is>
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>at least</t>
+          <t>park</t>
         </is>
       </c>
       <c r="C541" t="n">
@@ -8553,12 +8553,12 @@
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>täydellinen</t>
+          <t>seitsemän</t>
         </is>
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>perfect</t>
+          <t>seven</t>
         </is>
       </c>
       <c r="C542" t="n">
@@ -8568,12 +8568,12 @@
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>puisto</t>
+          <t>rouva</t>
         </is>
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>park</t>
+          <t>Ms.</t>
         </is>
       </c>
       <c r="C543" t="n">
@@ -8583,12 +8583,12 @@
     <row r="544">
       <c r="A544" t="inlineStr">
         <is>
-          <t>seitsemän</t>
+          <t>suo</t>
         </is>
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>seven</t>
+          <t>bog</t>
         </is>
       </c>
       <c r="C544" t="n">
@@ -8598,12 +8598,12 @@
     <row r="545">
       <c r="A545" t="inlineStr">
         <is>
-          <t>rouva</t>
+          <t>pihvi</t>
         </is>
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>Ms.</t>
+          <t>steak</t>
         </is>
       </c>
       <c r="C545" t="n">
@@ -8613,12 +8613,12 @@
     <row r="546">
       <c r="A546" t="inlineStr">
         <is>
-          <t>suo</t>
+          <t>poni</t>
         </is>
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>bog</t>
+          <t>pony</t>
         </is>
       </c>
       <c r="C546" t="n">
@@ -8628,12 +8628,12 @@
     <row r="547">
       <c r="A547" t="inlineStr">
         <is>
-          <t>pihvi</t>
+          <t>ketsuppi</t>
         </is>
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>steak</t>
+          <t>ketchup</t>
         </is>
       </c>
       <c r="C547" t="n">
@@ -8643,12 +8643,12 @@
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>poni</t>
+          <t>laulu</t>
         </is>
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>pony</t>
+          <t>song</t>
         </is>
       </c>
       <c r="C548" t="n">
@@ -8658,12 +8658,12 @@
     <row r="549">
       <c r="A549" t="inlineStr">
         <is>
-          <t>ketsuppi</t>
+          <t>seisoa</t>
         </is>
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>ketchup</t>
+          <t>to have stopped (clock, watch)</t>
         </is>
       </c>
       <c r="C549" t="n">
@@ -8673,12 +8673,12 @@
     <row r="550">
       <c r="A550" t="inlineStr">
         <is>
-          <t>laulu</t>
+          <t>muu</t>
         </is>
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>song</t>
+          <t>moo (cow sound)</t>
         </is>
       </c>
       <c r="C550" t="n">
@@ -8688,12 +8688,12 @@
     <row r="551">
       <c r="A551" t="inlineStr">
         <is>
-          <t>seisoa</t>
+          <t>tuoli</t>
         </is>
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>to have stopped (clock, watch)</t>
+          <t>chair</t>
         </is>
       </c>
       <c r="C551" t="n">
@@ -8703,12 +8703,12 @@
     <row r="552">
       <c r="A552" t="inlineStr">
         <is>
-          <t>muu</t>
+          <t>ratsastaa</t>
         </is>
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>moo (cow sound)</t>
+          <t>to ride (an animal)</t>
         </is>
       </c>
       <c r="C552" t="n">
@@ -8718,12 +8718,12 @@
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>tuoli</t>
+          <t>tiskata</t>
         </is>
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>chair</t>
+          <t>to do the dishes</t>
         </is>
       </c>
       <c r="C553" t="n">
@@ -8733,12 +8733,12 @@
     <row r="554">
       <c r="A554" t="inlineStr">
         <is>
-          <t>ratsastaa</t>
+          <t>surullinen</t>
         </is>
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>to ride (an animal)</t>
+          <t>sad</t>
         </is>
       </c>
       <c r="C554" t="n">
@@ -8748,12 +8748,12 @@
     <row r="555">
       <c r="A555" t="inlineStr">
         <is>
-          <t>tiskata</t>
+          <t>sanoa</t>
         </is>
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>to do the dishes</t>
+          <t>to say (some sound)</t>
         </is>
       </c>
       <c r="C555" t="n">
@@ -8763,12 +8763,12 @@
     <row r="556">
       <c r="A556" t="inlineStr">
         <is>
-          <t>surullinen</t>
+          <t>rauha</t>
         </is>
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>peace</t>
         </is>
       </c>
       <c r="C556" t="n">
@@ -8778,12 +8778,12 @@
     <row r="557">
       <c r="A557" t="inlineStr">
         <is>
-          <t>sanoa</t>
+          <t>munkki</t>
         </is>
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>to say (some sound)</t>
+          <t>jelly doughnut</t>
         </is>
       </c>
       <c r="C557" t="n">
@@ -8793,12 +8793,12 @@
     <row r="558">
       <c r="A558" t="inlineStr">
         <is>
-          <t>rauha</t>
+          <t>jäätelö</t>
         </is>
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>peace</t>
+          <t>ice cream</t>
         </is>
       </c>
       <c r="C558" t="n">
@@ -8808,12 +8808,12 @@
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>munkki</t>
+          <t>sinappi</t>
         </is>
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>jelly doughnut</t>
+          <t>mustard</t>
         </is>
       </c>
       <c r="C559" t="n">
@@ -8823,12 +8823,12 @@
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>jäätelö</t>
+          <t>teillä</t>
         </is>
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>ice cream</t>
+          <t>you (plural) have</t>
         </is>
       </c>
       <c r="C560" t="n">
@@ -8838,12 +8838,12 @@
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>sinappi</t>
+          <t>heillä</t>
         </is>
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>mustard</t>
+          <t>they have</t>
         </is>
       </c>
       <c r="C561" t="n">
@@ -8853,12 +8853,12 @@
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>teillä</t>
+          <t>nätti</t>
         </is>
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>you (plural) have</t>
+          <t>pretty (adjective)</t>
         </is>
       </c>
       <c r="C562" t="n">
@@ -8868,12 +8868,12 @@
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>heillä</t>
+          <t>sulhanen</t>
         </is>
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>they have</t>
+          <t>groom</t>
         </is>
       </c>
       <c r="C563" t="n">
@@ -8883,12 +8883,12 @@
     <row r="564">
       <c r="A564" t="inlineStr">
         <is>
-          <t>nätti</t>
+          <t>viineri</t>
         </is>
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>pretty (adjective)</t>
+          <t>Danish pastry</t>
         </is>
       </c>
       <c r="C564" t="n">
@@ -8898,31 +8898,31 @@
     <row r="565">
       <c r="A565" t="inlineStr">
         <is>
-          <t>sulhanen</t>
+          <t>insinööri</t>
         </is>
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>groom</t>
+          <t>engineer</t>
         </is>
       </c>
       <c r="C565" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="inlineStr">
         <is>
-          <t>viineri</t>
+          <t>liha</t>
         </is>
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>Danish pastry</t>
+          <t>meat</t>
         </is>
       </c>
       <c r="C566" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="567">

</xml_diff>